<commit_message>
switch example dataset from DRC to North America
</commit_message>
<xml_diff>
--- a/data-raw/geo_raw_example.xlsx
+++ b/data-raw/geo_raw_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/geomatch/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/hmatch/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8685BE6A-B5DC-ED41-BE94-77734DD7B76B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BF605-97BC-B442-AFC8-9BC6E23CF273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="9360" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
+    <workbookView xWindow="21540" yWindow="11360" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,78 +35,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>adm1</t>
   </si>
   <si>
-    <t>adm3</t>
-  </si>
-  <si>
     <t>adm2</t>
   </si>
   <si>
-    <t>adm4</t>
-  </si>
-  <si>
-    <t>Butembo</t>
-  </si>
-  <si>
-    <t>Ngule</t>
-  </si>
-  <si>
-    <t>Katwa</t>
-  </si>
-  <si>
-    <t>Makerere</t>
-  </si>
-  <si>
-    <t>Nord-Kivu</t>
-  </si>
-  <si>
-    <t>Katsya</t>
-  </si>
-  <si>
-    <t>Wayene</t>
-  </si>
-  <si>
-    <t>Vutetse</t>
-  </si>
-  <si>
-    <t>Kasongomi</t>
-  </si>
-  <si>
-    <t>Bagira</t>
-  </si>
-  <si>
-    <t>Mugaba</t>
-  </si>
-  <si>
-    <t>Vulindi</t>
-  </si>
-  <si>
-    <t>Lwamiso</t>
-  </si>
-  <si>
-    <t>Katwua</t>
-  </si>
-  <si>
-    <t>matando</t>
-  </si>
-  <si>
-    <t>matanda_ngule</t>
-  </si>
-  <si>
-    <t>butemba</t>
-  </si>
-  <si>
-    <t>nord kivu</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>Matanda</t>
+    <t>united states</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>suffolk</t>
+  </si>
+  <si>
+    <t>philadelphia</t>
+  </si>
+  <si>
+    <t>york</t>
+  </si>
+  <si>
+    <t>pensylvania</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>adm0</t>
+  </si>
+  <si>
+    <t>united_states</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>NJ_Bergen</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>York</t>
+  </si>
+  <si>
+    <t>philidelphia</t>
+  </si>
+  <si>
+    <t>jeffersen</t>
   </si>
 </sst>
 </file>
@@ -461,166 +452,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A42989-4AE2-0549-82CF-0E568F8D0EDB}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dictionary-recoding functionality, and revise/document match_type in hmatch_best()
</commit_message>
<xml_diff>
--- a/data-raw/geo_raw_example.xlsx
+++ b/data-raw/geo_raw_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/hmatch/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BF605-97BC-B442-AFC8-9BC6E23CF273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3146DF-0229-444F-A06C-76DD404CFD87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21540" yWindow="11360" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>york</t>
   </si>
   <si>
-    <t>pensylvania</t>
-  </si>
-  <si>
     <t>king</t>
   </si>
   <si>
@@ -88,16 +85,19 @@
     <t>NJ_Bergen</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>York</t>
   </si>
   <si>
-    <t>philidelphia</t>
-  </si>
-  <si>
     <t>jeffersen</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>Pensylvania</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -499,10 +499,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -518,10 +518,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -529,10 +529,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -540,10 +540,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,10 +551,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
internal refactor of hmatch_ fns to separate prep/string standardization from main matching routines, so that high-level fns can repeatedly call matching routines without having to repeat the time-consuming prep/standardization steps; also remove concise arg and add more unit tests
</commit_message>
<xml_diff>
--- a/data-raw/geo_raw_example.xlsx
+++ b/data-raw/geo_raw_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/hmatch/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3146DF-0229-444F-A06C-76DD404CFD87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A133C4-8A97-8C4D-B6A6-BC2AA3BB8BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="11360" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
+    <workbookView xWindow="19940" yWindow="8080" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>adm1</t>
   </si>
@@ -88,9 +88,6 @@
     <t>York</t>
   </si>
   <si>
-    <t>jeffersen</t>
-  </si>
-  <si>
     <t>Alameda</t>
   </si>
   <si>
@@ -98,6 +95,15 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Jeffersen</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A42989-4AE2-0549-82CF-0E568F8D0EDB}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -540,10 +546,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -570,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,6 +585,20 @@
       </c>
       <c r="D11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fn hmatch_permute and update example datasets to better illustrate various match types
</commit_message>
<xml_diff>
--- a/data-raw/geo_raw_example.xlsx
+++ b/data-raw/geo_raw_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbarks/hmatch/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A133C4-8A97-8C4D-B6A6-BC2AA3BB8BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C297FB9D-3A4D-4941-9918-58D0AC99EE41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19940" yWindow="8080" windowWidth="28040" windowHeight="17440" xr2:uid="{B5A821CA-BB04-F343-AEBE-7329BB64BC7D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>adm1</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Jeffersen</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
   </si>
 </sst>
 </file>
@@ -458,17 +464,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A42989-4AE2-0549-82CF-0E568F8D0EDB}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -575,8 +581,11 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -584,20 +593,28 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>